<commit_message>
generate objects from model0. 13970414
</commit_message>
<xml_diff>
--- a/logs_csv/pdfs/model7_laf_date_2018-06-19_12-23-39_epochs_100/model7_laf_date_2018-06-19_12-23-39__epochs_100_step_1.xlsx
+++ b/logs_csv/pdfs/model7_laf_date_2018-06-19_12-23-39_epochs_100/model7_laf_date_2018-06-19_12-23-39__epochs_100_step_1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>epoch</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>val_perplexity</t>
+  </si>
+  <si>
+    <t>min/max</t>
   </si>
 </sst>
 </file>
@@ -852,13 +855,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2337,6 +2348,27 @@
       </c>
       <c r="I51">
         <v>175.18511051864601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <f>MAX(B1:B51)</f>
+        <v>0.819716496462911</v>
+      </c>
+      <c r="C54">
+        <f>MIN(C1:C51)</f>
+        <v>0.63293163488339699</v>
+      </c>
+      <c r="F54">
+        <f>MAX(F1:F51)</f>
+        <v>0.79967500000000002</v>
+      </c>
+      <c r="H54">
+        <f>MIN(H1:H51)</f>
+        <v>0.72419553165435702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>